<commit_message>
Futsal World Cup 2016, AFrica Cup of Nations 1968
Futsal World Cup 2016 Groups A,B,C,D, AFrica Cup of Nations 1968
</commit_message>
<xml_diff>
--- a/Scripts/africacupofnations/africacupofnations.xlsx
+++ b/Scripts/africacupofnations/africacupofnations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="666" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="666" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="1957" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="1962" sheetId="89" r:id="rId3"/>
     <sheet name="1963" sheetId="90" r:id="rId4"/>
     <sheet name="1965" sheetId="91" r:id="rId5"/>
+    <sheet name="1968" sheetId="92" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -780,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="3">
-        <f t="shared" ref="B15:B18" si="4">B13</f>
+        <f t="shared" ref="B16:B18" si="4">B13</f>
         <v>2</v>
       </c>
       <c r="C16" s="3">
@@ -2339,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="3" t="str">
-        <f t="shared" ref="G20:G39" si="3">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A20 &amp; ", " &amp; B20 &amp; ", " &amp; C20 &amp; ", " &amp; D20 &amp; ", " &amp; E20 &amp; ", " &amp; F20 &amp; ");"</f>
+        <f t="shared" ref="G20:G35" si="3">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A20 &amp; ", " &amp; B20 &amp; ", " &amp; C20 &amp; ", " &amp; D20 &amp; ", " &amp; E20 &amp; ", " &amp; F20 &amp; ");"</f>
         <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (45, 11, 233, 1, 1, 2);</v>
       </c>
     </row>
@@ -2713,7 +2714,7 @@
         <v>60</v>
       </c>
       <c r="B35" s="4">
-        <f t="shared" ref="B35:B39" si="6">B32</f>
+        <f t="shared" ref="B35" si="6">B32</f>
         <v>14</v>
       </c>
       <c r="C35" s="4">
@@ -3158,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4449,4 +4450,2443 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="111.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>'1965'!A7+1</f>
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>1968</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>251</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <f>B2</f>
+        <v>1968</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>256</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <f>B3</f>
+        <v>1968</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>225</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>A4+1</f>
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f>B4</f>
+        <v>1968</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>213</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A5+1</f>
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <f>B5</f>
+        <v>1968</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>233</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A6+1</f>
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <f>B6</f>
+        <v>1968</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>221</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>A7+1</f>
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <f>B7</f>
+        <v>1968</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>2431</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <f>B8</f>
+        <v>1968</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>2422228</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="str">
+        <f>"insert into game (matchid, matchdate, game_type, country) values (" &amp; A11 &amp; ", '" &amp; B11 &amp; "', " &amp; C11 &amp; ", " &amp; D11 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (matchid, 'matchdate', game_type, country);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>'1965'!A17+1</f>
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>"1968-01-12"</f>
+        <v>1968-01-12</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>251</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" ref="G12:G27" si="0">"insert into game (matchid, matchdate, game_type, country) values (" &amp; A12 &amp; ", '" &amp; B12 &amp; "', " &amp; C12 &amp; ", " &amp; D12 &amp;  ");"</f>
+        <v>insert into game (matchid, matchdate, game_type, country) values (27, '1968-01-12', 2, 251);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A12+1</f>
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>"1968-01-12"</f>
+        <v>1968-01-12</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D27" si="1">D12</f>
+        <v>251</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (28, '1968-01-12', 2, 251);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" ref="A14:A27" si="2">A13+1</f>
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>"1968-01-14"</f>
+        <v>1968-01-14</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (29, '1968-01-14', 2, 251);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>"1968-01-14"</f>
+        <v>1968-01-14</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (30, '1968-01-14', 2, 251);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>"1968-01-16"</f>
+        <v>1968-01-16</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (31, '1968-01-16', 2, 251);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>"1968-01-16"</f>
+        <v>1968-01-16</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (32, '1968-01-16', 2, 251);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>"1968-01-12"</f>
+        <v>1968-01-12</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (33, '1968-01-12', 2, 251);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f>"1968-01-12"</f>
+        <v>1968-01-12</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (34, '1968-01-12', 2, 251);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>"1968-01-14"</f>
+        <v>1968-01-14</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (35, '1968-01-14', 2, 251);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>"1968-01-14"</f>
+        <v>1968-01-14</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (36, '1968-01-14', 2, 251);</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>"1968-01-16"</f>
+        <v>1968-01-16</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (37, '1968-01-16', 2, 251);</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>"1968-01-16"</f>
+        <v>1968-01-16</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (38, '1968-01-16', 2, 251);</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>"1968-01-19"</f>
+        <v>1968-01-19</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (39, '1968-01-19', 4, 251);</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>"1968-01-19"</f>
+        <v>1968-01-19</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (40, '1968-01-19', 4, 251);</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>"1968-01-21"</f>
+        <v>1968-01-21</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (41, '1968-01-21', 5, 251);</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>"1968-01-21"</f>
+        <v>1968-01-21</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>251</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into game (matchid, matchdate, game_type, country) values (42, '1968-01-21', 6, 251);</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="str">
+        <f>"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A29 &amp; ", " &amp; B29 &amp; ", " &amp; C29 &amp; ", " &amp; D29 &amp; ", " &amp; E29 &amp; ", " &amp; F29 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (id, matchid, squad, goals, points, time_type);</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <f>'1965'!A55 + 1</f>
+        <v>113</v>
+      </c>
+      <c r="B30" s="3">
+        <f>A12</f>
+        <v>27</v>
+      </c>
+      <c r="C30" s="3">
+        <v>251</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="str">
+        <f t="shared" ref="G30:G61" si="3">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A30 &amp; ", " &amp; B30 &amp; ", " &amp; C30 &amp; ", " &amp; D30 &amp; ", " &amp; E30 &amp; ", " &amp; F30 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (113, 27, 251, 2, 2, 2);</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f>A30+1</f>
+        <v>114</v>
+      </c>
+      <c r="B31" s="3">
+        <f>B30</f>
+        <v>27</v>
+      </c>
+      <c r="C31" s="3">
+        <v>251</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (114, 27, 251, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <f t="shared" ref="A32:A101" si="4">A31+1</f>
+        <v>115</v>
+      </c>
+      <c r="B32" s="3">
+        <f>B30</f>
+        <v>27</v>
+      </c>
+      <c r="C32" s="3">
+        <v>256</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (115, 27, 256, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <f t="shared" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="B33" s="3">
+        <f>B30</f>
+        <v>27</v>
+      </c>
+      <c r="C33" s="3">
+        <v>256</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
+        <v>1</v>
+      </c>
+      <c r="G33" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (116, 27, 256, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <f>A33+1</f>
+        <v>117</v>
+      </c>
+      <c r="B34" s="4">
+        <f>B30+1</f>
+        <v>28</v>
+      </c>
+      <c r="C34" s="4">
+        <v>225</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2</v>
+      </c>
+      <c r="F34" s="4">
+        <v>2</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (117, 28, 225, 3, 2, 2);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+      <c r="B35" s="4">
+        <f>B34</f>
+        <v>28</v>
+      </c>
+      <c r="C35" s="4">
+        <v>225</v>
+      </c>
+      <c r="D35" s="4">
+        <v>2</v>
+      </c>
+      <c r="E35" s="4">
+        <v>0</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (118, 28, 225, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <f t="shared" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="B36" s="4">
+        <f>B34</f>
+        <v>28</v>
+      </c>
+      <c r="C36" s="4">
+        <v>213</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>0</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (119, 28, 213, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+      <c r="B37" s="4">
+        <f>B34</f>
+        <v>28</v>
+      </c>
+      <c r="C37" s="4">
+        <v>213</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (120, 28, 213, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <f t="shared" si="4"/>
+        <v>121</v>
+      </c>
+      <c r="B38" s="3">
+        <f>B34+1</f>
+        <v>29</v>
+      </c>
+      <c r="C38" s="3">
+        <v>251</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1</v>
+      </c>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+      <c r="F38" s="3">
+        <v>2</v>
+      </c>
+      <c r="G38" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (121, 29, 251, 1, 2, 2);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <f t="shared" si="4"/>
+        <v>122</v>
+      </c>
+      <c r="B39" s="3">
+        <f>B38</f>
+        <v>29</v>
+      </c>
+      <c r="C39" s="3">
+        <v>251</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>1</v>
+      </c>
+      <c r="G39" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (122, 29, 251, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <f t="shared" si="4"/>
+        <v>123</v>
+      </c>
+      <c r="B40" s="3">
+        <f>B38</f>
+        <v>29</v>
+      </c>
+      <c r="C40" s="3">
+        <v>225</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2</v>
+      </c>
+      <c r="G40" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (123, 29, 225, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <f t="shared" si="4"/>
+        <v>124</v>
+      </c>
+      <c r="B41" s="3">
+        <f t="shared" ref="B41" si="5">B38</f>
+        <v>29</v>
+      </c>
+      <c r="C41" s="3">
+        <v>225</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0</v>
+      </c>
+      <c r="F41" s="3">
+        <v>1</v>
+      </c>
+      <c r="G41" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (124, 29, 225, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <f t="shared" si="4"/>
+        <v>125</v>
+      </c>
+      <c r="B42" s="4">
+        <f>B38+1</f>
+        <v>30</v>
+      </c>
+      <c r="C42" s="4">
+        <v>213</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2</v>
+      </c>
+      <c r="F42" s="4">
+        <v>2</v>
+      </c>
+      <c r="G42" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (125, 30, 213, 1, 2, 2);</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <f t="shared" si="4"/>
+        <v>126</v>
+      </c>
+      <c r="B43" s="4">
+        <f>B42</f>
+        <v>30</v>
+      </c>
+      <c r="C43" s="4">
+        <v>213</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1</v>
+      </c>
+      <c r="G43" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (126, 30, 213, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <f t="shared" si="4"/>
+        <v>127</v>
+      </c>
+      <c r="B44" s="4">
+        <f>B42</f>
+        <v>30</v>
+      </c>
+      <c r="C44" s="4">
+        <v>256</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>2</v>
+      </c>
+      <c r="G44" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (127, 30, 256, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="B45" s="4">
+        <f t="shared" ref="B45" si="6">B42</f>
+        <v>30</v>
+      </c>
+      <c r="C45" s="4">
+        <v>256</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0</v>
+      </c>
+      <c r="F45" s="4">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (128, 30, 256, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <f t="shared" si="4"/>
+        <v>129</v>
+      </c>
+      <c r="B46" s="3">
+        <f>B42+1</f>
+        <v>31</v>
+      </c>
+      <c r="C46" s="3">
+        <v>225</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3">
+        <v>2</v>
+      </c>
+      <c r="G46" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (129, 31, 225, 2, 2, 2);</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
+      <c r="B47" s="3">
+        <f>B46</f>
+        <v>31</v>
+      </c>
+      <c r="C47" s="3">
+        <v>225</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
+      <c r="F47" s="3">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (130, 31, 225, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <f t="shared" si="4"/>
+        <v>131</v>
+      </c>
+      <c r="B48" s="3">
+        <f>B46</f>
+        <v>31</v>
+      </c>
+      <c r="C48" s="3">
+        <v>256</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2</v>
+      </c>
+      <c r="G48" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (131, 31, 256, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+      <c r="B49" s="3">
+        <f t="shared" ref="B49" si="7">B46</f>
+        <v>31</v>
+      </c>
+      <c r="C49" s="3">
+        <v>256</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
+        <v>1</v>
+      </c>
+      <c r="G49" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (132, 31, 256, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <f t="shared" si="4"/>
+        <v>133</v>
+      </c>
+      <c r="B50" s="4">
+        <f>B46+1</f>
+        <v>32</v>
+      </c>
+      <c r="C50" s="4">
+        <v>251</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2</v>
+      </c>
+      <c r="F50" s="4">
+        <v>2</v>
+      </c>
+      <c r="G50" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (133, 32, 251, 3, 2, 2);</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <f t="shared" si="4"/>
+        <v>134</v>
+      </c>
+      <c r="B51" s="4">
+        <f>B50</f>
+        <v>32</v>
+      </c>
+      <c r="C51" s="4">
+        <v>251</v>
+      </c>
+      <c r="D51" s="4">
+        <v>3</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0</v>
+      </c>
+      <c r="F51" s="4">
+        <v>1</v>
+      </c>
+      <c r="G51" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (134, 32, 251, 3, 0, 1);</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <f t="shared" si="4"/>
+        <v>135</v>
+      </c>
+      <c r="B52" s="4">
+        <f>B50</f>
+        <v>32</v>
+      </c>
+      <c r="C52" s="4">
+        <v>213</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="F52" s="4">
+        <v>2</v>
+      </c>
+      <c r="G52" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (135, 32, 213, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
+      <c r="B53" s="4">
+        <f t="shared" ref="B53" si="8">B50</f>
+        <v>32</v>
+      </c>
+      <c r="C53" s="4">
+        <v>213</v>
+      </c>
+      <c r="D53" s="4">
+        <v>0</v>
+      </c>
+      <c r="E53" s="4">
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (136, 32, 213, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <f t="shared" si="4"/>
+        <v>137</v>
+      </c>
+      <c r="B54" s="3">
+        <f>B50+1</f>
+        <v>33</v>
+      </c>
+      <c r="C54" s="3">
+        <v>233</v>
+      </c>
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <v>2</v>
+      </c>
+      <c r="G54" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (137, 33, 233, 2, 1, 2);</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+      <c r="B55" s="3">
+        <f>B54</f>
+        <v>33</v>
+      </c>
+      <c r="C55" s="3">
+        <v>233</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (138, 33, 233, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <f t="shared" si="4"/>
+        <v>139</v>
+      </c>
+      <c r="B56" s="3">
+        <f>B54</f>
+        <v>33</v>
+      </c>
+      <c r="C56" s="3">
+        <v>221</v>
+      </c>
+      <c r="D56" s="3">
+        <v>2</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (139, 33, 221, 2, 1, 2);</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="B57" s="3">
+        <f t="shared" ref="B57" si="9">B54</f>
+        <v>33</v>
+      </c>
+      <c r="C57" s="3">
+        <v>221</v>
+      </c>
+      <c r="D57" s="3">
+        <v>1</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (140, 33, 221, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <f t="shared" si="4"/>
+        <v>141</v>
+      </c>
+      <c r="B58" s="4">
+        <f>B54+1</f>
+        <v>34</v>
+      </c>
+      <c r="C58" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D58" s="4">
+        <v>3</v>
+      </c>
+      <c r="E58" s="4">
+        <v>2</v>
+      </c>
+      <c r="F58" s="4">
+        <v>2</v>
+      </c>
+      <c r="G58" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (141, 34, 2431, 3, 2, 2);</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <f t="shared" si="4"/>
+        <v>142</v>
+      </c>
+      <c r="B59" s="4">
+        <f>B58</f>
+        <v>34</v>
+      </c>
+      <c r="C59" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D59" s="4">
+        <v>2</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>1</v>
+      </c>
+      <c r="G59" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (142, 34, 2431, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="B60" s="4">
+        <f>B58</f>
+        <v>34</v>
+      </c>
+      <c r="C60" s="4">
+        <v>2422228</v>
+      </c>
+      <c r="D60" s="4">
+        <v>0</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <v>2</v>
+      </c>
+      <c r="G60" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (143, 34, 2422228, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+      <c r="B61" s="4">
+        <f t="shared" ref="B61" si="10">B58</f>
+        <v>34</v>
+      </c>
+      <c r="C61" s="4">
+        <v>2422228</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4">
+        <v>0</v>
+      </c>
+      <c r="F61" s="4">
+        <v>1</v>
+      </c>
+      <c r="G61" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (144, 34, 2422228, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <f t="shared" si="4"/>
+        <v>145</v>
+      </c>
+      <c r="B62" s="3">
+        <f>B58+1</f>
+        <v>35</v>
+      </c>
+      <c r="C62" s="3">
+        <v>221</v>
+      </c>
+      <c r="D62" s="3">
+        <v>2</v>
+      </c>
+      <c r="E62" s="3">
+        <v>2</v>
+      </c>
+      <c r="F62" s="3">
+        <v>2</v>
+      </c>
+      <c r="G62" s="3" t="str">
+        <f t="shared" ref="G62:G101" si="11">"insert into game_score (id, matchid, squad, goals, points, time_type) values (" &amp; A62 &amp; ", " &amp; B62 &amp; ", " &amp; C62 &amp; ", " &amp; D62 &amp; ", " &amp; E62 &amp; ", " &amp; F62 &amp; ");"</f>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (145, 35, 221, 2, 2, 2);</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
+      <c r="B63" s="3">
+        <f>B62</f>
+        <v>35</v>
+      </c>
+      <c r="C63" s="3">
+        <v>221</v>
+      </c>
+      <c r="D63" s="3">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3">
+        <v>0</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (146, 35, 221, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <f t="shared" si="4"/>
+        <v>147</v>
+      </c>
+      <c r="B64" s="3">
+        <f>B62</f>
+        <v>35</v>
+      </c>
+      <c r="C64" s="3">
+        <v>2422228</v>
+      </c>
+      <c r="D64" s="3">
+        <v>1</v>
+      </c>
+      <c r="E64" s="3">
+        <v>0</v>
+      </c>
+      <c r="F64" s="3">
+        <v>2</v>
+      </c>
+      <c r="G64" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (147, 35, 2422228, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+      <c r="B65" s="3">
+        <f t="shared" ref="B65" si="12">B62</f>
+        <v>35</v>
+      </c>
+      <c r="C65" s="3">
+        <v>2422228</v>
+      </c>
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (148, 35, 2422228, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <f t="shared" si="4"/>
+        <v>149</v>
+      </c>
+      <c r="B66" s="4">
+        <f>B62+1</f>
+        <v>36</v>
+      </c>
+      <c r="C66" s="4">
+        <v>233</v>
+      </c>
+      <c r="D66" s="4">
+        <v>2</v>
+      </c>
+      <c r="E66" s="4">
+        <v>2</v>
+      </c>
+      <c r="F66" s="4">
+        <v>2</v>
+      </c>
+      <c r="G66" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (149, 36, 233, 2, 2, 2);</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="B67" s="4">
+        <f>B66</f>
+        <v>36</v>
+      </c>
+      <c r="C67" s="4">
+        <v>233</v>
+      </c>
+      <c r="D67" s="4">
+        <v>1</v>
+      </c>
+      <c r="E67" s="4">
+        <v>0</v>
+      </c>
+      <c r="F67" s="4">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (150, 36, 233, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <f t="shared" si="4"/>
+        <v>151</v>
+      </c>
+      <c r="B68" s="4">
+        <f>B66</f>
+        <v>36</v>
+      </c>
+      <c r="C68" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D68" s="4">
+        <v>1</v>
+      </c>
+      <c r="E68" s="4">
+        <v>0</v>
+      </c>
+      <c r="F68" s="4">
+        <v>2</v>
+      </c>
+      <c r="G68" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (151, 36, 2431, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+      <c r="B69" s="4">
+        <f t="shared" ref="B69" si="13">B66</f>
+        <v>36</v>
+      </c>
+      <c r="C69" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="4">
+        <v>0</v>
+      </c>
+      <c r="F69" s="4">
+        <v>1</v>
+      </c>
+      <c r="G69" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (152, 36, 2431, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <f t="shared" si="4"/>
+        <v>153</v>
+      </c>
+      <c r="B70" s="3">
+        <f>B66+1</f>
+        <v>37</v>
+      </c>
+      <c r="C70" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D70" s="3">
+        <v>2</v>
+      </c>
+      <c r="E70" s="3">
+        <v>2</v>
+      </c>
+      <c r="F70" s="3">
+        <v>2</v>
+      </c>
+      <c r="G70" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (153, 37, 2431, 2, 2, 2);</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="B71" s="3">
+        <f>B70</f>
+        <v>37</v>
+      </c>
+      <c r="C71" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" s="3">
+        <v>0</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (154, 37, 2431, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <f t="shared" si="4"/>
+        <v>155</v>
+      </c>
+      <c r="B72" s="3">
+        <f>B70</f>
+        <v>37</v>
+      </c>
+      <c r="C72" s="3">
+        <v>221</v>
+      </c>
+      <c r="D72" s="3">
+        <v>1</v>
+      </c>
+      <c r="E72" s="3">
+        <v>0</v>
+      </c>
+      <c r="F72" s="3">
+        <v>2</v>
+      </c>
+      <c r="G72" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (155, 37, 221, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+      <c r="B73" s="3">
+        <f t="shared" ref="B73" si="14">B70</f>
+        <v>37</v>
+      </c>
+      <c r="C73" s="3">
+        <v>221</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="3">
+        <v>0</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1</v>
+      </c>
+      <c r="G73" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (156, 37, 221, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <f t="shared" si="4"/>
+        <v>157</v>
+      </c>
+      <c r="B74" s="4">
+        <f>B70+1</f>
+        <v>38</v>
+      </c>
+      <c r="C74" s="4">
+        <v>233</v>
+      </c>
+      <c r="D74" s="4">
+        <v>3</v>
+      </c>
+      <c r="E74" s="4">
+        <v>2</v>
+      </c>
+      <c r="F74" s="4">
+        <v>2</v>
+      </c>
+      <c r="G74" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (157, 38, 233, 3, 2, 2);</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+      <c r="B75" s="4">
+        <f>B74</f>
+        <v>38</v>
+      </c>
+      <c r="C75" s="4">
+        <v>233</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" s="4">
+        <v>0</v>
+      </c>
+      <c r="F75" s="4">
+        <v>1</v>
+      </c>
+      <c r="G75" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (158, 38, 233, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <f t="shared" si="4"/>
+        <v>159</v>
+      </c>
+      <c r="B76" s="4">
+        <f>B74</f>
+        <v>38</v>
+      </c>
+      <c r="C76" s="4">
+        <v>2422228</v>
+      </c>
+      <c r="D76" s="4">
+        <v>1</v>
+      </c>
+      <c r="E76" s="4">
+        <v>0</v>
+      </c>
+      <c r="F76" s="4">
+        <v>2</v>
+      </c>
+      <c r="G76" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (159, 38, 2422228, 1, 0, 2);</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="B77" s="4">
+        <f t="shared" ref="B77" si="15">B74</f>
+        <v>38</v>
+      </c>
+      <c r="C77" s="4">
+        <v>2422228</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="4">
+        <v>0</v>
+      </c>
+      <c r="F77" s="4">
+        <v>1</v>
+      </c>
+      <c r="G77" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (160, 38, 2422228, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <f t="shared" si="4"/>
+        <v>161</v>
+      </c>
+      <c r="B78" s="3">
+        <f>B74+1</f>
+        <v>39</v>
+      </c>
+      <c r="C78" s="3">
+        <v>251</v>
+      </c>
+      <c r="D78" s="3">
+        <v>2</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>2</v>
+      </c>
+      <c r="G78" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (161, 39, 251, 2, 0, 2);</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+      <c r="B79" s="3">
+        <f>B78</f>
+        <v>39</v>
+      </c>
+      <c r="C79" s="3">
+        <v>261</v>
+      </c>
+      <c r="D79" s="3">
+        <v>1</v>
+      </c>
+      <c r="E79" s="3">
+        <v>0</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1</v>
+      </c>
+      <c r="G79" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (162, 39, 261, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <f t="shared" si="4"/>
+        <v>163</v>
+      </c>
+      <c r="B80" s="3">
+        <f>B78</f>
+        <v>39</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D80" s="3">
+        <v>2</v>
+      </c>
+      <c r="E80" s="3">
+        <v>0</v>
+      </c>
+      <c r="F80" s="3">
+        <v>2</v>
+      </c>
+      <c r="G80" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (163, 39, 2431, 2, 0, 2);</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <f t="shared" si="4"/>
+        <v>164</v>
+      </c>
+      <c r="B81" s="3">
+        <f t="shared" ref="B81:B85" si="16">B78</f>
+        <v>39</v>
+      </c>
+      <c r="C81" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D81" s="3">
+        <v>2</v>
+      </c>
+      <c r="E81" s="3">
+        <v>0</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (164, 39, 2431, 2, 0, 1);</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <f t="shared" si="4"/>
+        <v>165</v>
+      </c>
+      <c r="B82" s="3">
+        <f t="shared" si="16"/>
+        <v>39</v>
+      </c>
+      <c r="C82" s="3">
+        <v>251</v>
+      </c>
+      <c r="D82" s="3">
+        <v>2</v>
+      </c>
+      <c r="E82" s="3">
+        <v>0</v>
+      </c>
+      <c r="F82" s="3">
+        <v>4</v>
+      </c>
+      <c r="G82" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (165, 39, 251, 2, 0, 4);</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+      <c r="B83" s="3">
+        <f t="shared" si="16"/>
+        <v>39</v>
+      </c>
+      <c r="C83" s="3">
+        <v>261</v>
+      </c>
+      <c r="D83" s="3">
+        <v>2</v>
+      </c>
+      <c r="E83" s="3">
+        <v>0</v>
+      </c>
+      <c r="F83" s="3">
+        <v>3</v>
+      </c>
+      <c r="G83" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (166, 39, 261, 2, 0, 3);</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <f t="shared" si="4"/>
+        <v>167</v>
+      </c>
+      <c r="B84" s="3">
+        <f t="shared" si="16"/>
+        <v>39</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D84" s="3">
+        <v>3</v>
+      </c>
+      <c r="E84" s="3">
+        <v>2</v>
+      </c>
+      <c r="F84" s="3">
+        <v>4</v>
+      </c>
+      <c r="G84" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (167, 39, 2431, 3, 2, 4);</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <f t="shared" si="4"/>
+        <v>168</v>
+      </c>
+      <c r="B85" s="3">
+        <f t="shared" si="16"/>
+        <v>39</v>
+      </c>
+      <c r="C85" s="3">
+        <v>2431</v>
+      </c>
+      <c r="D85" s="3">
+        <v>3</v>
+      </c>
+      <c r="E85" s="3">
+        <v>2</v>
+      </c>
+      <c r="F85" s="3">
+        <v>3</v>
+      </c>
+      <c r="G85" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (168, 39, 2431, 3, 2, 3);</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <f t="shared" si="4"/>
+        <v>169</v>
+      </c>
+      <c r="B86" s="4">
+        <f>B78+1</f>
+        <v>40</v>
+      </c>
+      <c r="C86" s="4">
+        <v>233</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" s="4">
+        <v>0</v>
+      </c>
+      <c r="F86" s="4">
+        <v>2</v>
+      </c>
+      <c r="G86" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (169, 40, 233, null, 0, 2);</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="B87" s="4">
+        <f>B86</f>
+        <v>40</v>
+      </c>
+      <c r="C87" s="4">
+        <v>233</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" s="4">
+        <v>0</v>
+      </c>
+      <c r="F87" s="4">
+        <v>1</v>
+      </c>
+      <c r="G87" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (170, 40, 233, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="4">
+        <f t="shared" si="4"/>
+        <v>171</v>
+      </c>
+      <c r="B88" s="4">
+        <f>B86</f>
+        <v>40</v>
+      </c>
+      <c r="C88" s="4">
+        <v>225</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" s="4">
+        <v>0</v>
+      </c>
+      <c r="F88" s="4">
+        <v>2</v>
+      </c>
+      <c r="G88" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (171, 40, 225, null, 0, 2);</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <f t="shared" si="4"/>
+        <v>172</v>
+      </c>
+      <c r="B89" s="4">
+        <f t="shared" ref="B89:B93" si="17">B86</f>
+        <v>40</v>
+      </c>
+      <c r="C89" s="4">
+        <v>225</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" s="4">
+        <v>0</v>
+      </c>
+      <c r="F89" s="4">
+        <v>1</v>
+      </c>
+      <c r="G89" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (172, 40, 225, null, 0, 1);</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <f t="shared" si="4"/>
+        <v>173</v>
+      </c>
+      <c r="B90" s="4">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="C90" s="4">
+        <v>233</v>
+      </c>
+      <c r="D90" s="4">
+        <v>4</v>
+      </c>
+      <c r="E90" s="4">
+        <v>2</v>
+      </c>
+      <c r="F90" s="4">
+        <v>4</v>
+      </c>
+      <c r="G90" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (173, 40, 233, 4, 2, 4);</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+      <c r="B91" s="4">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="C91" s="4">
+        <v>233</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="4">
+        <v>0</v>
+      </c>
+      <c r="F91" s="4">
+        <v>3</v>
+      </c>
+      <c r="G91" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (174, 40, 233, null, 0, 3);</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <f t="shared" si="4"/>
+        <v>175</v>
+      </c>
+      <c r="B92" s="4">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="C92" s="4">
+        <v>225</v>
+      </c>
+      <c r="D92" s="4">
+        <v>3</v>
+      </c>
+      <c r="E92" s="4">
+        <v>0</v>
+      </c>
+      <c r="F92" s="4">
+        <v>4</v>
+      </c>
+      <c r="G92" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (175, 40, 225, 3, 0, 4);</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <f t="shared" si="4"/>
+        <v>176</v>
+      </c>
+      <c r="B93" s="4">
+        <f t="shared" si="17"/>
+        <v>40</v>
+      </c>
+      <c r="C93" s="4">
+        <v>225</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" s="4">
+        <v>0</v>
+      </c>
+      <c r="F93" s="4">
+        <v>3</v>
+      </c>
+      <c r="G93" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (176, 40, 225, null, 0, 3);</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <f t="shared" si="4"/>
+        <v>177</v>
+      </c>
+      <c r="B94" s="3">
+        <f>B86+1</f>
+        <v>41</v>
+      </c>
+      <c r="C94" s="3">
+        <v>225</v>
+      </c>
+      <c r="D94" s="3">
+        <v>1</v>
+      </c>
+      <c r="E94" s="3">
+        <v>2</v>
+      </c>
+      <c r="F94" s="3">
+        <v>2</v>
+      </c>
+      <c r="G94" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (177, 41, 225, 1, 2, 2);</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <f t="shared" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="B95" s="3">
+        <f>B94</f>
+        <v>41</v>
+      </c>
+      <c r="C95" s="3">
+        <v>225</v>
+      </c>
+      <c r="D95" s="3">
+        <v>1</v>
+      </c>
+      <c r="E95" s="3">
+        <v>0</v>
+      </c>
+      <c r="F95" s="3">
+        <v>1</v>
+      </c>
+      <c r="G95" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (178, 41, 225, 1, 0, 1);</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <f t="shared" si="4"/>
+        <v>179</v>
+      </c>
+      <c r="B96" s="3">
+        <f>B94</f>
+        <v>41</v>
+      </c>
+      <c r="C96" s="3">
+        <v>251</v>
+      </c>
+      <c r="D96" s="3">
+        <v>0</v>
+      </c>
+      <c r="E96" s="3">
+        <v>0</v>
+      </c>
+      <c r="F96" s="3">
+        <v>2</v>
+      </c>
+      <c r="G96" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (179, 41, 251, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="B97" s="3">
+        <f t="shared" ref="B97" si="18">B94</f>
+        <v>41</v>
+      </c>
+      <c r="C97" s="3">
+        <v>251</v>
+      </c>
+      <c r="D97" s="3">
+        <v>0</v>
+      </c>
+      <c r="E97" s="3">
+        <v>0</v>
+      </c>
+      <c r="F97" s="3">
+        <v>1</v>
+      </c>
+      <c r="G97" s="3" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (180, 41, 251, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <f t="shared" si="4"/>
+        <v>181</v>
+      </c>
+      <c r="B98" s="4">
+        <f>B94+1</f>
+        <v>42</v>
+      </c>
+      <c r="C98" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D98" s="4">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4">
+        <v>2</v>
+      </c>
+      <c r="F98" s="4">
+        <v>2</v>
+      </c>
+      <c r="G98" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (181, 42, 2431, 1, 2, 2);</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+      <c r="B99" s="4">
+        <f>B98</f>
+        <v>42</v>
+      </c>
+      <c r="C99" s="4">
+        <v>2431</v>
+      </c>
+      <c r="D99" s="4">
+        <v>0</v>
+      </c>
+      <c r="E99" s="4">
+        <v>0</v>
+      </c>
+      <c r="F99" s="4">
+        <v>1</v>
+      </c>
+      <c r="G99" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (182, 42, 2431, 0, 0, 1);</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <f t="shared" si="4"/>
+        <v>183</v>
+      </c>
+      <c r="B100" s="4">
+        <f>B98</f>
+        <v>42</v>
+      </c>
+      <c r="C100" s="4">
+        <v>233</v>
+      </c>
+      <c r="D100" s="4">
+        <v>0</v>
+      </c>
+      <c r="E100" s="4">
+        <v>0</v>
+      </c>
+      <c r="F100" s="4">
+        <v>2</v>
+      </c>
+      <c r="G100" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (183, 42, 233, 0, 0, 2);</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <f t="shared" si="4"/>
+        <v>184</v>
+      </c>
+      <c r="B101" s="4">
+        <f t="shared" ref="B101" si="19">B98</f>
+        <v>42</v>
+      </c>
+      <c r="C101" s="4">
+        <v>233</v>
+      </c>
+      <c r="D101" s="4">
+        <v>0</v>
+      </c>
+      <c r="E101" s="4">
+        <v>0</v>
+      </c>
+      <c r="F101" s="4">
+        <v>1</v>
+      </c>
+      <c r="G101" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>insert into game_score (id, matchid, squad, goals, points, time_type) values (184, 42, 233, 0, 0, 1);</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>